<commit_message>
version con transiciones de video
</commit_message>
<xml_diff>
--- a/Backend/gesture_sequence.xlsx
+++ b/Backend/gesture_sequence.xlsx
@@ -451,7 +451,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -461,7 +461,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -471,7 +471,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -481,7 +481,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -491,7 +491,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -511,7 +511,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -521,7 +521,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -551,7 +551,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -561,7 +561,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -611,7 +611,7 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -651,7 +651,7 @@
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -681,7 +681,7 @@
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -691,7 +691,7 @@
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -701,7 +701,7 @@
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -711,7 +711,7 @@
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -731,7 +731,7 @@
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -761,7 +761,7 @@
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -771,7 +771,7 @@
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -821,7 +821,7 @@
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -881,7 +881,7 @@
       </c>
       <c r="B45" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -901,7 +901,7 @@
       </c>
       <c r="B47" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -911,7 +911,7 @@
       </c>
       <c r="B48" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -921,7 +921,7 @@
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -961,7 +961,7 @@
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -971,7 +971,7 @@
       </c>
       <c r="B54" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -1001,7 +1001,7 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1021,7 +1021,7 @@
       </c>
       <c r="B59" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="B60" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1051,7 +1051,7 @@
       </c>
       <c r="B62" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1081,7 +1081,7 @@
       </c>
       <c r="B65" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -1101,7 +1101,7 @@
       </c>
       <c r="B67" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -1111,7 +1111,7 @@
       </c>
       <c r="B68" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -1121,7 +1121,7 @@
       </c>
       <c r="B69" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1151,7 +1151,7 @@
       </c>
       <c r="B72" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -1161,7 +1161,7 @@
       </c>
       <c r="B73" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -1221,7 +1221,7 @@
       </c>
       <c r="B79" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1251,7 +1251,7 @@
       </c>
       <c r="B82" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1261,7 +1261,7 @@
       </c>
       <c r="B83" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1271,7 +1271,7 @@
       </c>
       <c r="B84" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1371,7 +1371,7 @@
       </c>
       <c r="B94" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -1381,7 +1381,7 @@
       </c>
       <c r="B95" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -1421,7 +1421,7 @@
       </c>
       <c r="B99" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1431,7 +1431,7 @@
       </c>
       <c r="B100" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1441,7 +1441,7 @@
       </c>
       <c r="B101" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1451,7 +1451,7 @@
       </c>
       <c r="B102" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1461,7 +1461,7 @@
       </c>
       <c r="B103" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1471,7 +1471,7 @@
       </c>
       <c r="B104" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1481,7 +1481,7 @@
       </c>
       <c r="B105" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1491,7 +1491,7 @@
       </c>
       <c r="B106" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1501,7 +1501,7 @@
       </c>
       <c r="B107" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1511,7 +1511,7 @@
       </c>
       <c r="B108" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1521,7 +1521,7 @@
       </c>
       <c r="B109" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1531,7 +1531,7 @@
       </c>
       <c r="B110" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1541,7 +1541,7 @@
       </c>
       <c r="B111" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1551,7 +1551,7 @@
       </c>
       <c r="B112" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1671,7 +1671,7 @@
       </c>
       <c r="B124" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1801,7 +1801,7 @@
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1841,7 +1841,7 @@
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1871,7 +1871,7 @@
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1881,7 +1881,7 @@
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1951,7 +1951,7 @@
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -1981,7 +1981,7 @@
       </c>
       <c r="B155" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2001,7 +2001,7 @@
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2061,7 +2061,7 @@
       </c>
       <c r="B163" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2121,7 +2121,7 @@
       </c>
       <c r="B169" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2131,7 +2131,7 @@
       </c>
       <c r="B170" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2141,7 +2141,7 @@
       </c>
       <c r="B171" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -2181,7 +2181,7 @@
       </c>
       <c r="B175" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -2191,7 +2191,7 @@
       </c>
       <c r="B176" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -2241,7 +2241,7 @@
       </c>
       <c r="B181" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -2261,7 +2261,7 @@
       </c>
       <c r="B183" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -2281,7 +2281,7 @@
       </c>
       <c r="B185" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2331,7 +2331,7 @@
       </c>
       <c r="B190" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2341,7 +2341,7 @@
       </c>
       <c r="B191" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2351,7 +2351,7 @@
       </c>
       <c r="B192" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2361,7 +2361,7 @@
       </c>
       <c r="B193" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2371,7 +2371,7 @@
       </c>
       <c r="B194" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2381,7 +2381,7 @@
       </c>
       <c r="B195" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2391,7 +2391,7 @@
       </c>
       <c r="B196" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2401,7 +2401,7 @@
       </c>
       <c r="B197" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2411,7 +2411,7 @@
       </c>
       <c r="B198" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2421,7 +2421,7 @@
       </c>
       <c r="B199" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2431,7 +2431,7 @@
       </c>
       <c r="B200" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2471,7 +2471,7 @@
       </c>
       <c r="B204" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2491,7 +2491,7 @@
       </c>
       <c r="B206" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2541,7 +2541,7 @@
       </c>
       <c r="B211" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,7 @@
       </c>
       <c r="B222" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -2661,7 +2661,7 @@
       </c>
       <c r="B223" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -2671,7 +2671,7 @@
       </c>
       <c r="B224" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -2681,7 +2681,7 @@
       </c>
       <c r="B225" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -2691,7 +2691,7 @@
       </c>
       <c r="B226" t="inlineStr">
         <is>
-          <t>Attention</t>
+          <t>EyesClosed</t>
         </is>
       </c>
     </row>
@@ -2711,7 +2711,7 @@
       </c>
       <c r="B228" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2721,7 +2721,7 @@
       </c>
       <c r="B229" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2731,7 +2731,7 @@
       </c>
       <c r="B230" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2741,7 +2741,7 @@
       </c>
       <c r="B231" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2751,7 +2751,7 @@
       </c>
       <c r="B232" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2761,7 +2761,7 @@
       </c>
       <c r="B233" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2811,7 +2811,7 @@
       </c>
       <c r="B238" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2821,7 +2821,7 @@
       </c>
       <c r="B239" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>
@@ -2841,7 +2841,7 @@
       </c>
       <c r="B241" t="inlineStr">
         <is>
-          <t>EyesClosed</t>
+          <t>Attention</t>
         </is>
       </c>
     </row>

</xml_diff>